<commit_message>
R data files creates from data-processing script
</commit_message>
<xml_diff>
--- a/2016-Opening1.xlsx
+++ b/2016-Opening1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/VikasMaturi1/Autumn-2019/COMM177b/rising-waters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E96FFCAF-C687-7444-9F19-80AFC52FE2A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6B507E-BF76-2344-918A-C9C24A1544BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{4F6BFCD2-CD0F-6F4E-BEC8-894FA084BD96}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" xr2:uid="{4F6BFCD2-CD0F-6F4E-BEC8-894FA084BD96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -45,57 +45,33 @@
     <t>CFS</t>
   </si>
   <si>
-    <t>    </t>
-  </si>
-  <si>
-    <t>Day 1</t>
-  </si>
-  <si>
     <t>Jan. 10</t>
   </si>
   <si>
-    <t>Day 2</t>
-  </si>
-  <si>
     <t>Jan. 11</t>
   </si>
   <si>
-    <t>Day 3</t>
-  </si>
-  <si>
     <t>Jan. 12</t>
   </si>
   <si>
-    <t>Day 4</t>
-  </si>
-  <si>
     <t>Jan. 13</t>
   </si>
   <si>
     <t>30       </t>
   </si>
   <si>
-    <t>Day 5</t>
-  </si>
-  <si>
     <t>Jan. 14 </t>
   </si>
   <si>
     <t>100 </t>
   </si>
   <si>
-    <t>Day 6</t>
-  </si>
-  <si>
     <t> Jan. 15</t>
   </si>
   <si>
     <t>130 </t>
   </si>
   <si>
-    <t>Day 7</t>
-  </si>
-  <si>
     <t> Jan. 16</t>
   </si>
   <si>
@@ -105,24 +81,15 @@
     <t>196,000 </t>
   </si>
   <si>
-    <t>Day 8</t>
-  </si>
-  <si>
     <t> Jan. 17</t>
   </si>
   <si>
     <t>210 </t>
   </si>
   <si>
-    <t>Day 9</t>
-  </si>
-  <si>
     <t> Jan. 18</t>
   </si>
   <si>
-    <t>Day 10</t>
-  </si>
-  <si>
     <t> Jan. 19</t>
   </si>
   <si>
@@ -132,85 +99,49 @@
     <t>201,000 </t>
   </si>
   <si>
-    <t>Day 11</t>
-  </si>
-  <si>
     <t>Jan. 20</t>
   </si>
   <si>
-    <t>Day 12</t>
-  </si>
-  <si>
     <t>Jan. 21</t>
   </si>
   <si>
-    <t>Day 13</t>
-  </si>
-  <si>
     <t>Jan. 22</t>
   </si>
   <si>
-    <t>Day 14</t>
-  </si>
-  <si>
     <t>Jan. 23</t>
   </si>
   <si>
-    <t>Day 15</t>
-  </si>
-  <si>
     <t>Jan. 24</t>
   </si>
   <si>
-    <t>Day 16</t>
-  </si>
-  <si>
     <t>Jan. 25</t>
   </si>
   <si>
-    <t>Day 17</t>
-  </si>
-  <si>
     <t>Jan. 26</t>
   </si>
   <si>
-    <t>Day 18</t>
-  </si>
-  <si>
     <t>Jan. 27</t>
   </si>
   <si>
-    <t>Day 19</t>
-  </si>
-  <si>
     <t>Jan. 28</t>
   </si>
   <si>
-    <t>Day 20</t>
-  </si>
-  <si>
     <t>Jan. 29</t>
   </si>
   <si>
-    <t>Day 21</t>
-  </si>
-  <si>
     <t>Jan. 30</t>
   </si>
   <si>
     <t>57 </t>
   </si>
   <si>
-    <t>Day 22</t>
-  </si>
-  <si>
     <t>Jan. 31</t>
   </si>
   <si>
-    <t>Day 23</t>
-  </si>
-  <si>
     <t>Feb. 1</t>
+  </si>
+  <si>
+    <t>Day</t>
   </si>
 </sst>
 </file>
@@ -580,35 +511,35 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="18">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="18">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>20</v>
@@ -623,11 +554,11 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="18">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
+      <c r="A3" s="2">
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>18</v>
@@ -642,11 +573,11 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="18">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
+      <c r="A4" s="2">
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>22</v>
@@ -661,14 +592,14 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="18">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
+      <c r="A5" s="2">
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
         <v>90</v>
@@ -680,17 +611,17 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="18">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
+      <c r="A6" s="2">
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E6" s="3">
         <v>104000</v>
@@ -699,17 +630,17 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
+      <c r="A7" s="2">
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2">
         <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3">
         <v>132000</v>
@@ -718,36 +649,36 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="18">
-      <c r="A8" s="2" t="s">
-        <v>20</v>
+      <c r="A8" s="2">
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2">
         <v>52</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="18">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
+      <c r="A9" s="2">
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2">
         <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3">
         <v>203000</v>
@@ -756,17 +687,17 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="18">
-      <c r="A10" s="2" t="s">
-        <v>27</v>
+      <c r="A10" s="2">
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E10" s="3">
         <v>201000</v>
@@ -775,30 +706,30 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="18">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
+      <c r="A11" s="2">
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="18">
-      <c r="A12" s="2" t="s">
-        <v>33</v>
+      <c r="A12" s="2">
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -813,11 +744,11 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="18">
-      <c r="A13" s="2" t="s">
-        <v>35</v>
+      <c r="A13" s="2">
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -832,11 +763,11 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="18">
-      <c r="A14" s="2" t="s">
-        <v>37</v>
+      <c r="A14" s="2">
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
@@ -851,11 +782,11 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="18">
-      <c r="A15" s="2" t="s">
-        <v>39</v>
+      <c r="A15" s="2">
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -870,11 +801,11 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="18">
-      <c r="A16" s="2" t="s">
-        <v>41</v>
+      <c r="A16" s="2">
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2">
         <v>0</v>
@@ -889,11 +820,11 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="18">
-      <c r="A17" s="2" t="s">
-        <v>43</v>
+      <c r="A17" s="2">
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2">
         <v>-13</v>
@@ -908,11 +839,11 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="18">
-      <c r="A18" s="2" t="s">
-        <v>45</v>
+      <c r="A18" s="2">
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2">
         <v>-20</v>
@@ -927,11 +858,11 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="18">
-      <c r="A19" s="2" t="s">
-        <v>47</v>
+      <c r="A19" s="2">
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C19" s="2">
         <v>-22</v>
@@ -946,11 +877,11 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="18">
-      <c r="A20" s="2" t="s">
-        <v>49</v>
+      <c r="A20" s="2">
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C20" s="2">
         <v>-24</v>
@@ -965,11 +896,11 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="18">
-      <c r="A21" s="2" t="s">
-        <v>51</v>
+      <c r="A21" s="2">
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C21" s="2">
         <v>-40</v>
@@ -984,17 +915,17 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="18">
-      <c r="A22" s="2" t="s">
-        <v>53</v>
+      <c r="A22" s="2">
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C22" s="2">
         <v>-34</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="E22" s="3">
         <v>30000</v>
@@ -1003,11 +934,11 @@
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="18">
-      <c r="A23" s="2" t="s">
-        <v>56</v>
+      <c r="A23" s="2">
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2">
         <v>-33</v>
@@ -1022,11 +953,11 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" ht="18">
-      <c r="A24" s="2" t="s">
-        <v>58</v>
+      <c r="A24" s="2">
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2">
         <v>-24</v>

</xml_diff>